<commit_message>
Update Kaggle challenge, House Prices - Advanced Regression Techniques; Working on data analysis
</commit_message>
<xml_diff>
--- a/challenges/02_HousePricesCompetition/whatExpect.xlsx
+++ b/challenges/02_HousePricesCompetition/whatExpect.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$E$80</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -93,9 +93,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Building (Physical caracteristics)
-Space (Properties of house)
-Location (Information about the place where house is located)</t>
+Our expectation about the variable influence in 'SalePrice'. We can use a categorical scale with 'High', 'Medium' and 'Low' as possible values.</t>
         </r>
       </text>
     </comment>
@@ -119,35 +117,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Our expectation about the variable influence in 'SalePrice'. We can use a categorical scale with 'High', 'Medium' and 'Low' as possible values.</t>
+Our conclusions about the importance of the variable, after we give a quick look at the data. We can keep with the same categorical scale as in 'Expectation'.</t>
         </r>
       </text>
     </comment>
     <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Our conclusions about the importance of the variable, after we give a quick look at the data. We can keep with the same categorical scale as in 'Expectation'.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="162">
   <si>
     <t>Variable</t>
   </si>
@@ -184,9 +158,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Segment</t>
-  </si>
-  <si>
     <t>Expectation</t>
   </si>
   <si>
@@ -202,9 +173,6 @@
     <t>Numerical</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -232,20 +200,449 @@
     <t>Lot size in square feet</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Street</t>
   </si>
   <si>
     <t>Type of road access</t>
+  </si>
+  <si>
+    <t>Alley</t>
+  </si>
+  <si>
+    <t>Many missing values</t>
+  </si>
+  <si>
+    <t>LotShape</t>
+  </si>
+  <si>
+    <t>LandContour</t>
+  </si>
+  <si>
+    <t>all categories have houses with all kinds of values</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>it only has a value that is different from the others</t>
+  </si>
+  <si>
+    <t>LotConfig</t>
+  </si>
+  <si>
+    <t>LandSlope</t>
+  </si>
+  <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
+    <t>The neighborhood seems to have little influence on the value of houses.</t>
+  </si>
+  <si>
+    <t>Condition1</t>
+  </si>
+  <si>
+    <t>Proximity to main road or railroad</t>
+  </si>
+  <si>
+    <t>Condition2</t>
+  </si>
+  <si>
+    <t>BldgType</t>
+  </si>
+  <si>
+    <t>Type of dwelling</t>
+  </si>
+  <si>
+    <t>HouseStyle</t>
+  </si>
+  <si>
+    <t>Style of dwelling</t>
+  </si>
+  <si>
+    <t>OverallQual</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Overall material and finish quality</t>
+  </si>
+  <si>
+    <t>OverallCond</t>
+  </si>
+  <si>
+    <t>Overall condition rating</t>
+  </si>
+  <si>
+    <t>YearBuilt</t>
+  </si>
+  <si>
+    <t>Original construction date</t>
+  </si>
+  <si>
+    <t>YearRemodAdd</t>
+  </si>
+  <si>
+    <t>Remodel date</t>
+  </si>
+  <si>
+    <t>RoofStyle</t>
+  </si>
+  <si>
+    <t>Type of roof</t>
+  </si>
+  <si>
+    <t>RoofMatl</t>
+  </si>
+  <si>
+    <t>Roof material</t>
+  </si>
+  <si>
+    <t>Exterior1st</t>
+  </si>
+  <si>
+    <t>Exterior2nd</t>
+  </si>
+  <si>
+    <t>MasVnrType</t>
+  </si>
+  <si>
+    <t>Exterior covering on house</t>
+  </si>
+  <si>
+    <t>Exterior covering on house (if more than one material)</t>
+  </si>
+  <si>
+    <t>Masonry veneer type</t>
+  </si>
+  <si>
+    <t>MasVnrArea</t>
+  </si>
+  <si>
+    <t>Masonry veneer area in square feet</t>
+  </si>
+  <si>
+    <t>ExterQual</t>
+  </si>
+  <si>
+    <t>Exterior material quality</t>
+  </si>
+  <si>
+    <t>ExterCond</t>
+  </si>
+  <si>
+    <t>Present condition of the material on the exterior</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>Type of foundation</t>
+  </si>
+  <si>
+    <t>BsmtQual</t>
+  </si>
+  <si>
+    <t>Height of the basement</t>
+  </si>
+  <si>
+    <t>BsmtCond</t>
+  </si>
+  <si>
+    <t>General condition of the basement</t>
+  </si>
+  <si>
+    <t>BsmtExposure</t>
+  </si>
+  <si>
+    <t>Walkout or garden level basement walls</t>
+  </si>
+  <si>
+    <t>BsmtFinSF1</t>
+  </si>
+  <si>
+    <t>Type 1 finished square feet</t>
+  </si>
+  <si>
+    <t>BsmtFinType1</t>
+  </si>
+  <si>
+    <t>Quality of basement finished area</t>
+  </si>
+  <si>
+    <t>BsmtFinType2</t>
+  </si>
+  <si>
+    <t>BsmtFinSF2</t>
+  </si>
+  <si>
+    <t>Type 2 finished square feet</t>
+  </si>
+  <si>
+    <t>BsmtUnfSF</t>
+  </si>
+  <si>
+    <t>Unfinished square feet of basement area</t>
+  </si>
+  <si>
+    <t>TotalBsmtSF</t>
+  </si>
+  <si>
+    <t>Total square feet of basement area</t>
+  </si>
+  <si>
+    <t>Heating</t>
+  </si>
+  <si>
+    <t>Type of heating</t>
+  </si>
+  <si>
+    <t>HeatingQC</t>
+  </si>
+  <si>
+    <t>Quality of Heating</t>
+  </si>
+  <si>
+    <t>CentralAir</t>
+  </si>
+  <si>
+    <t>Central air conditioning</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Electrical system</t>
+  </si>
+  <si>
+    <t>1stFlrSF</t>
+  </si>
+  <si>
+    <t>2ndFlrSF</t>
+  </si>
+  <si>
+    <t>First Floor square feet</t>
+  </si>
+  <si>
+    <t>Second Floor square feet</t>
+  </si>
+  <si>
+    <t>LowQualFinSF</t>
+  </si>
+  <si>
+    <t>Low quality finished square feet (all floors)</t>
+  </si>
+  <si>
+    <t>GrLivArea</t>
+  </si>
+  <si>
+    <t>Above grade (ground) living area square feet</t>
+  </si>
+  <si>
+    <t>BsmtFullBath</t>
+  </si>
+  <si>
+    <t>Basement full bathrooms</t>
+  </si>
+  <si>
+    <t>BsmtHalfBath</t>
+  </si>
+  <si>
+    <t>Basement half bathrooms</t>
+  </si>
+  <si>
+    <t>FullBath</t>
+  </si>
+  <si>
+    <t>Full bathrooms above grade</t>
+  </si>
+  <si>
+    <t>HalfBath</t>
+  </si>
+  <si>
+    <t>Half bathrooms above grade</t>
+  </si>
+  <si>
+    <t>BedroomAbvGr</t>
+  </si>
+  <si>
+    <t>KitchenAbvGr</t>
+  </si>
+  <si>
+    <t>Number of kitchens</t>
+  </si>
+  <si>
+    <t>Number of bedrooms above basement level</t>
+  </si>
+  <si>
+    <t>KitchenQual</t>
+  </si>
+  <si>
+    <t>Total rooms above grade (does not include bathrooms)</t>
+  </si>
+  <si>
+    <t>TotRmsAbvGrd</t>
+  </si>
+  <si>
+    <t>Kitchen quality</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Fireplaces</t>
+  </si>
+  <si>
+    <t>Home functionality rating</t>
+  </si>
+  <si>
+    <t>Number of fireplaces</t>
+  </si>
+  <si>
+    <t>FireplaceQu</t>
+  </si>
+  <si>
+    <t>Fireplace Quality, but many missing values</t>
+  </si>
+  <si>
+    <t>GarageType</t>
+  </si>
+  <si>
+    <t>Garage location</t>
+  </si>
+  <si>
+    <t>GarageYrBlt</t>
+  </si>
+  <si>
+    <t>GarageFinish</t>
+  </si>
+  <si>
+    <t>GarageCars</t>
+  </si>
+  <si>
+    <t>GarageArea</t>
+  </si>
+  <si>
+    <t>GarageQual</t>
+  </si>
+  <si>
+    <t>GarageCond</t>
+  </si>
+  <si>
+    <t>Year garage was built</t>
+  </si>
+  <si>
+    <t>Interior finish of the garage</t>
+  </si>
+  <si>
+    <t>Size of garage in car capacity</t>
+  </si>
+  <si>
+    <t>Size of garage in square feet</t>
+  </si>
+  <si>
+    <t>Garage quality</t>
+  </si>
+  <si>
+    <t>Garage condition</t>
+  </si>
+  <si>
+    <t>Paved driveway</t>
+  </si>
+  <si>
+    <t>PavedDrive</t>
+  </si>
+  <si>
+    <t>WoodDeckSF</t>
+  </si>
+  <si>
+    <t>Wood deck area in square feet</t>
+  </si>
+  <si>
+    <t>Open porch area in square feet</t>
+  </si>
+  <si>
+    <t>OpenPorchSF</t>
+  </si>
+  <si>
+    <t>Enclosed porch area in square feet</t>
+  </si>
+  <si>
+    <t>EnclosedPorch</t>
+  </si>
+  <si>
+    <t>3SsnPorch</t>
+  </si>
+  <si>
+    <t>Three season porch area in square feet</t>
+  </si>
+  <si>
+    <t>ScreenPorch</t>
+  </si>
+  <si>
+    <t>Screen porch area in square feet</t>
+  </si>
+  <si>
+    <t>PoolArea</t>
+  </si>
+  <si>
+    <t>PoolQC</t>
+  </si>
+  <si>
+    <t>Fence quality</t>
+  </si>
+  <si>
+    <t>Fence</t>
+  </si>
+  <si>
+    <t>Pool quality</t>
+  </si>
+  <si>
+    <t>Pool area in square feet</t>
+  </si>
+  <si>
+    <t>MiscFeature</t>
+  </si>
+  <si>
+    <t>Miscellaneous feature not covered in other categories</t>
+  </si>
+  <si>
+    <t>MiscVal</t>
+  </si>
+  <si>
+    <t>MoSold</t>
+  </si>
+  <si>
+    <t>YrSold</t>
+  </si>
+  <si>
+    <t>SaleType</t>
+  </si>
+  <si>
+    <t>SaleCondition</t>
+  </si>
+  <si>
+    <t>$Value of miscellaneous feature</t>
+  </si>
+  <si>
+    <t>Month Sold</t>
+  </si>
+  <si>
+    <t>Year Sold</t>
+  </si>
+  <si>
+    <t>Type of sale</t>
+  </si>
+  <si>
+    <t>Condition of sale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +675,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -287,7 +695,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -295,14 +703,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,123 +1034,1234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" hidden="1">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" hidden="1">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1">
+      <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1">
+      <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1">
+      <c r="A12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1">
+      <c r="A15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1">
+      <c r="A19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" hidden="1">
+      <c r="A23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" hidden="1">
+      <c r="A24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" hidden="1">
+      <c r="A25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="29" spans="1:5" hidden="1">
+      <c r="A29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" hidden="1">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1">
+      <c r="A31" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1">
+      <c r="A32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" hidden="1">
+      <c r="A33" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1">
+      <c r="A34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D35" s="1"/>
+      <c r="E35" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
+    </row>
+    <row r="36" spans="1:5" hidden="1">
+      <c r="A36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1">
+      <c r="A37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1">
+      <c r="A38" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1">
+      <c r="A40" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1">
+      <c r="A41" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" hidden="1">
+      <c r="A46" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" hidden="1">
+      <c r="A48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1">
+      <c r="A49" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1">
+      <c r="A51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1">
+      <c r="A52" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1">
+      <c r="A53" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" hidden="1">
+      <c r="A54" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" hidden="1">
+      <c r="A56" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" hidden="1">
+      <c r="A57" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" hidden="1">
+      <c r="A58" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" hidden="1">
+      <c r="A59" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" hidden="1">
+      <c r="A60" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" hidden="1">
+      <c r="A61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" hidden="1">
+      <c r="A64" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" hidden="1">
+      <c r="A65" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" hidden="1">
+      <c r="A66" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" hidden="1">
+      <c r="A67" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" hidden="1">
+      <c r="A68" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" hidden="1">
+      <c r="A69" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" hidden="1">
+      <c r="A70" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" hidden="1">
+      <c r="A71" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" hidden="1">
+      <c r="A72" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" hidden="1">
+      <c r="A73" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" hidden="1">
+      <c r="A74" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" hidden="1">
+      <c r="A75" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" hidden="1">
+      <c r="A76" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" hidden="1">
+      <c r="A77" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" hidden="1">
+      <c r="A78" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" hidden="1">
+      <c r="A79" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" hidden="1">
+      <c r="A80" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:E80">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="High"/>
+        <filter val="Medium"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A4:E63">
+      <sortCondition ref="C1:C80"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -733,7 +2274,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -745,7 +2286,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>